<commit_message>
wardoslo, wardbergen, wardtrondheim, wardstavanger
</commit_message>
<xml_diff>
--- a/inst/rawdata/locations/norway_locations_ward.xlsx
+++ b/inst/rawdata/locations/norway_locations_ward.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riwh\OneDrive - Folkehelseinstituttet\packages\fhidata\inst\rawdata\locations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="13_ncr:1_{E0AA4139-EC72-7240-B4DA-8072FE8D2BA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A8D1A11-8AC8-4201-98D7-569D4DE6B1BB}"/>
+  <xr:revisionPtr revIDLastSave="281" documentId="13_ncr:1_{E0AA4139-EC72-7240-B4DA-8072FE8D2BA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{CF263F48-793B-4A56-AA49-F16A88F83BD9}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2205" windowWidth="20550" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="norwayLocations" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="117">
   <si>
     <t>year_start</t>
   </si>
@@ -150,33 +150,6 @@
     <t>municip0301</t>
   </si>
   <si>
-    <t>ward110301</t>
-  </si>
-  <si>
-    <t>ward110302</t>
-  </si>
-  <si>
-    <t>ward110303</t>
-  </si>
-  <si>
-    <t>ward110304</t>
-  </si>
-  <si>
-    <t>ward110305</t>
-  </si>
-  <si>
-    <t>ward110306</t>
-  </si>
-  <si>
-    <t>ward110307</t>
-  </si>
-  <si>
-    <t>ward110308</t>
-  </si>
-  <si>
-    <t>ward110309</t>
-  </si>
-  <si>
     <t>Hundvåg</t>
   </si>
   <si>
@@ -210,30 +183,6 @@
     <t>Stavanger</t>
   </si>
   <si>
-    <t>ward120101</t>
-  </si>
-  <si>
-    <t>ward120102</t>
-  </si>
-  <si>
-    <t>ward120103</t>
-  </si>
-  <si>
-    <t>ward120104</t>
-  </si>
-  <si>
-    <t>ward120105</t>
-  </si>
-  <si>
-    <t>ward120106</t>
-  </si>
-  <si>
-    <t>ward120107</t>
-  </si>
-  <si>
-    <t>ward120108</t>
-  </si>
-  <si>
     <t>Arna</t>
   </si>
   <si>
@@ -264,45 +213,9 @@
     <t>Bergen</t>
   </si>
   <si>
-    <t>ward460101</t>
-  </si>
-  <si>
-    <t>ward460102</t>
-  </si>
-  <si>
-    <t>ward460103</t>
-  </si>
-  <si>
-    <t>ward460104</t>
-  </si>
-  <si>
-    <t>ward460105</t>
-  </si>
-  <si>
-    <t>ward460106</t>
-  </si>
-  <si>
-    <t>ward460107</t>
-  </si>
-  <si>
-    <t>ward460108</t>
-  </si>
-  <si>
     <t>municip4601</t>
   </si>
   <si>
-    <t>ward160101</t>
-  </si>
-  <si>
-    <t>ward160102</t>
-  </si>
-  <si>
-    <t>ward160103</t>
-  </si>
-  <si>
-    <t>ward160104</t>
-  </si>
-  <si>
     <t>Midtbyen</t>
   </si>
   <si>
@@ -321,19 +234,151 @@
     <t>Trondheim</t>
   </si>
   <si>
-    <t>ward500101</t>
-  </si>
-  <si>
-    <t>ward500102</t>
-  </si>
-  <si>
-    <t>ward500103</t>
-  </si>
-  <si>
-    <t>ward500104</t>
-  </si>
-  <si>
     <t>municip5001</t>
+  </si>
+  <si>
+    <t>wardstavanger110301</t>
+  </si>
+  <si>
+    <t>wardstavanger110302</t>
+  </si>
+  <si>
+    <t>wardstavanger110303</t>
+  </si>
+  <si>
+    <t>wardstavanger110304</t>
+  </si>
+  <si>
+    <t>wardstavanger110305</t>
+  </si>
+  <si>
+    <t>wardstavanger110306</t>
+  </si>
+  <si>
+    <t>wardstavanger110307</t>
+  </si>
+  <si>
+    <t>wardstavanger110308</t>
+  </si>
+  <si>
+    <t>wardstavanger110309</t>
+  </si>
+  <si>
+    <t>wardbergen460101</t>
+  </si>
+  <si>
+    <t>wardbergen460102</t>
+  </si>
+  <si>
+    <t>wardbergen460103</t>
+  </si>
+  <si>
+    <t>wardbergen460104</t>
+  </si>
+  <si>
+    <t>wardbergen460105</t>
+  </si>
+  <si>
+    <t>wardbergen460106</t>
+  </si>
+  <si>
+    <t>wardbergen460107</t>
+  </si>
+  <si>
+    <t>wardbergen460108</t>
+  </si>
+  <si>
+    <t>wardbergen120101</t>
+  </si>
+  <si>
+    <t>wardbergen120102</t>
+  </si>
+  <si>
+    <t>wardbergen120103</t>
+  </si>
+  <si>
+    <t>wardbergen120104</t>
+  </si>
+  <si>
+    <t>wardbergen120105</t>
+  </si>
+  <si>
+    <t>wardbergen120106</t>
+  </si>
+  <si>
+    <t>wardbergen120107</t>
+  </si>
+  <si>
+    <t>wardbergen120108</t>
+  </si>
+  <si>
+    <t>wardtrondheim500101</t>
+  </si>
+  <si>
+    <t>wardtrondheim500102</t>
+  </si>
+  <si>
+    <t>wardtrondheim500103</t>
+  </si>
+  <si>
+    <t>wardtrondheim500104</t>
+  </si>
+  <si>
+    <t>wardtrondheim160101</t>
+  </si>
+  <si>
+    <t>wardtrondheim160102</t>
+  </si>
+  <si>
+    <t>wardtrondheim160103</t>
+  </si>
+  <si>
+    <t>wardtrondheim160104</t>
+  </si>
+  <si>
+    <t>wardoslo030101</t>
+  </si>
+  <si>
+    <t>wardoslo030102</t>
+  </si>
+  <si>
+    <t>wardoslo030103</t>
+  </si>
+  <si>
+    <t>wardoslo030104</t>
+  </si>
+  <si>
+    <t>wardoslo030105</t>
+  </si>
+  <si>
+    <t>wardoslo030106</t>
+  </si>
+  <si>
+    <t>wardoslo030107</t>
+  </si>
+  <si>
+    <t>wardoslo030108</t>
+  </si>
+  <si>
+    <t>wardoslo030109</t>
+  </si>
+  <si>
+    <t>wardoslo030110</t>
+  </si>
+  <si>
+    <t>wardoslo030111</t>
+  </si>
+  <si>
+    <t>wardoslo030112</t>
+  </si>
+  <si>
+    <t>wardoslo030113</t>
+  </si>
+  <si>
+    <t>wardoslo030114</t>
+  </si>
+  <si>
+    <t>wardoslo030115</t>
   </si>
 </sst>
 </file>
@@ -698,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +754,7 @@
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="3" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
@@ -1002,16 +1047,16 @@
         <v>2005</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1019,16 +1064,16 @@
         <v>2005</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H18" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1036,16 +1081,16 @@
         <v>2005</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H19" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1053,16 +1098,16 @@
         <v>2005</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H20" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1070,16 +1115,16 @@
         <v>2005</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H21" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1087,16 +1132,16 @@
         <v>2005</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H22" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1104,16 +1149,16 @@
         <v>2005</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H23" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1121,16 +1166,16 @@
         <v>2005</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H24" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1138,336 +1183,294 @@
         <v>2005</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="F25" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H25" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2005</v>
       </c>
-      <c r="B26" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C26" t="s">
-        <v>78</v>
-      </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="F26" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="H26" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2005</v>
       </c>
-      <c r="B27" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
       <c r="E27" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="H27" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2005</v>
       </c>
-      <c r="B28" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C28" t="s">
-        <v>80</v>
-      </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="F28" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="G28" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="H28" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2005</v>
       </c>
-      <c r="B29" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C29" t="s">
-        <v>81</v>
-      </c>
       <c r="E29" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="F29" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="G29" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="H29" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2005</v>
       </c>
-      <c r="B30" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C30" t="s">
-        <v>82</v>
-      </c>
       <c r="E30" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="F30" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="H30" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2005</v>
       </c>
-      <c r="B31" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C31" t="s">
-        <v>83</v>
-      </c>
       <c r="E31" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="F31" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="G31" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="H31" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2005</v>
       </c>
-      <c r="B32" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C32" t="s">
-        <v>84</v>
-      </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="G32" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="H32" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2005</v>
       </c>
-      <c r="B33" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>67</v>
+      <c r="E33" t="s">
+        <v>70</v>
       </c>
       <c r="F33" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="G33" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="H33" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F34" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="G34" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="H34" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F35" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="G35" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="H35" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F36" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="H36" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F37" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="G37" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="H37" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F38" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="G38" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="H38" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="E39" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F39" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="G39" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="H39" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="E40" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F40" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="G40" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="H40" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>85</v>
+        <v>2005</v>
+      </c>
+      <c r="B41" s="3">
+        <v>2019</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" t="s">
+        <v>86</v>
       </c>
       <c r="F41" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G41" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="H41" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1475,22 +1478,22 @@
         <v>2005</v>
       </c>
       <c r="B42" s="3">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="E42" t="s">
         <v>87</v>
       </c>
       <c r="F42" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="G42" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="H42" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1498,22 +1501,22 @@
         <v>2005</v>
       </c>
       <c r="B43" s="3">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E43" t="s">
         <v>88</v>
       </c>
       <c r="F43" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="G43" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="H43" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1521,22 +1524,22 @@
         <v>2005</v>
       </c>
       <c r="B44" s="3">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C44" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E44" t="s">
         <v>89</v>
       </c>
       <c r="F44" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="G44" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="H44" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1544,90 +1547,387 @@
         <v>2005</v>
       </c>
       <c r="B45" s="3">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C45" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="E45" t="s">
         <v>90</v>
       </c>
       <c r="F45" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="G45" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="H45" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>2018</v>
+        <v>2005</v>
+      </c>
+      <c r="B46" s="3">
+        <v>2019</v>
+      </c>
+      <c r="C46" t="s">
+        <v>83</v>
       </c>
       <c r="E46" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F46" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="G46" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="H46" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>2018</v>
+        <v>2005</v>
+      </c>
+      <c r="B47" s="3">
+        <v>2019</v>
+      </c>
+      <c r="C47" t="s">
+        <v>84</v>
       </c>
       <c r="E47" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F47" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="G47" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="H47" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>2018</v>
-      </c>
-      <c r="E48" t="s">
-        <v>99</v>
+        <v>2005</v>
+      </c>
+      <c r="B48" s="3">
+        <v>2019</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="F48" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="G48" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="H48" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E49" t="s">
+        <v>78</v>
+      </c>
+      <c r="F49" t="s">
+        <v>51</v>
+      </c>
+      <c r="G49" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E50" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50" t="s">
+        <v>52</v>
+      </c>
+      <c r="G50" t="s">
+        <v>61</v>
+      </c>
+      <c r="H50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E51" t="s">
+        <v>80</v>
+      </c>
+      <c r="F51" t="s">
+        <v>53</v>
+      </c>
+      <c r="G51" t="s">
+        <v>61</v>
+      </c>
+      <c r="H51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E52" t="s">
+        <v>81</v>
+      </c>
+      <c r="F52" t="s">
+        <v>54</v>
+      </c>
+      <c r="G52" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E53" t="s">
+        <v>82</v>
+      </c>
+      <c r="F53" t="s">
+        <v>55</v>
+      </c>
+      <c r="G53" t="s">
+        <v>61</v>
+      </c>
+      <c r="H53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E54" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" t="s">
+        <v>56</v>
+      </c>
+      <c r="G54" t="s">
+        <v>61</v>
+      </c>
+      <c r="H54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E55" t="s">
+        <v>84</v>
+      </c>
+      <c r="F55" t="s">
+        <v>57</v>
+      </c>
+      <c r="G55" t="s">
+        <v>61</v>
+      </c>
+      <c r="H55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F56" t="s">
+        <v>58</v>
+      </c>
+      <c r="G56" t="s">
+        <v>61</v>
+      </c>
+      <c r="H56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B57" s="3">
+        <v>2017</v>
+      </c>
+      <c r="C57" t="s">
+        <v>94</v>
+      </c>
+      <c r="E57" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" t="s">
+        <v>62</v>
+      </c>
+      <c r="G57" t="s">
+        <v>66</v>
+      </c>
+      <c r="H57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B58" s="3">
+        <v>2017</v>
+      </c>
+      <c r="C58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" t="s">
+        <v>99</v>
+      </c>
+      <c r="F58" t="s">
+        <v>63</v>
+      </c>
+      <c r="G58" t="s">
+        <v>66</v>
+      </c>
+      <c r="H58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B59" s="3">
+        <v>2017</v>
+      </c>
+      <c r="C59" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59" t="s">
+        <v>100</v>
+      </c>
+      <c r="F59" t="s">
+        <v>64</v>
+      </c>
+      <c r="G59" t="s">
+        <v>66</v>
+      </c>
+      <c r="H59" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B60" s="3">
+        <v>2017</v>
+      </c>
+      <c r="C60" t="s">
+        <v>97</v>
+      </c>
+      <c r="E60" t="s">
+        <v>101</v>
+      </c>
+      <c r="F60" t="s">
+        <v>65</v>
+      </c>
+      <c r="G60" t="s">
+        <v>66</v>
+      </c>
+      <c r="H60" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>2018</v>
       </c>
-      <c r="E49" t="s">
-        <v>100</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="E61" t="s">
         <v>94</v>
       </c>
-      <c r="G49" t="s">
-        <v>101</v>
-      </c>
-      <c r="H49" t="s">
+      <c r="F61" t="s">
+        <v>62</v>
+      </c>
+      <c r="G61" t="s">
+        <v>68</v>
+      </c>
+      <c r="H61" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E62" t="s">
+        <v>95</v>
+      </c>
+      <c r="F62" t="s">
+        <v>63</v>
+      </c>
+      <c r="G62" t="s">
+        <v>68</v>
+      </c>
+      <c r="H62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E63" t="s">
         <v>96</v>
+      </c>
+      <c r="F63" t="s">
+        <v>64</v>
+      </c>
+      <c r="G63" t="s">
+        <v>68</v>
+      </c>
+      <c r="H63" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E64" t="s">
+        <v>97</v>
+      </c>
+      <c r="F64" t="s">
+        <v>65</v>
+      </c>
+      <c r="G64" t="s">
+        <v>68</v>
+      </c>
+      <c r="H64" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>